<commit_message>
retire ":" dans freq
</commit_message>
<xml_diff>
--- a/resultats.xlsx
+++ b/resultats.xlsx
@@ -8,32 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Cours\FI3\S6\PROJ631\MiniProjet2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6943AD9-3AFC-4F8A-8B1E-D2EA49A7247B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC6990-59C1-4744-8F6C-996C0CBFC87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-13755" windowWidth="29040" windowHeight="16440" xr2:uid="{4FF68D20-8D89-47CC-9305-1CB8CE16F315}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4FF68D20-8D89-47CC-9305-1CB8CE16F315}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$A$2:$A$6</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Feuil1!$D$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Feuil1!$D$2:$D$6</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Feuil1!$B$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Feuil1!$B$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Feuil1!$B$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Feuil1!$B$5:$F$5</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Feuil1!$B$6:$F$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$B$2:$B$6</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$B$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$B$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$B$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$B$5:$F$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$B$6:$F$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Feuil1!$C$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Feuil1!$C$2:$C$6</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -527,19 +508,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>-3.4443999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-6.5</c:v>
+                  <c:v>-4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.6389</c:v>
+                  <c:v>-1.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40450000000000003</c:v>
+                  <c:v>0.41539999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43819999999999998</c:v>
+                  <c:v>0.43919999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,7 +707,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Feuil1!$C$1</c15:sqref>
@@ -789,7 +770,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -811,7 +792,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Feuil1!$A$2:$A$6</c15:sqref>
@@ -840,7 +821,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Feuil1!$C$2:$C$6</c15:sqref>
@@ -868,7 +849,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-A0BF-4B39-841A-0647FAE2C2A3}"/>
                   </c:ext>
@@ -881,7 +862,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Feuil1!$D$1</c15:sqref>
@@ -944,7 +925,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -966,7 +947,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Feuil1!$A$2:$A$6</c15:sqref>
@@ -995,7 +976,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Feuil1!$D$2:$D$6</c15:sqref>
@@ -1006,24 +987,24 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>50</c:v>
+                        <c:v>36</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>29</c:v>
+                        <c:v>21</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>114</c:v>
+                        <c:v>82</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>538</c:v>
+                        <c:v>406</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>651</c:v>
+                        <c:v>507</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-A0BF-4B39-841A-0647FAE2C2A3}"/>
                   </c:ext>
@@ -1293,6 +1274,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1A78-4B55-9066-003D17B389F2}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1308,6 +1294,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1A78-4B55-9066-003D17B389F2}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1323,6 +1314,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1A78-4B55-9066-003D17B389F2}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1354,7 +1350,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1536,6 +1532,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1054-4541-9504-64EF35ED726C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1551,6 +1552,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1054-4541-9504-64EF35ED726C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1566,6 +1572,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1054-4541-9504-64EF35ED726C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1597,7 +1608,7 @@
                   <c:v>84787</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>651</c:v>
+                  <c:v>507</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,7 +1620,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3797,7 +3807,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F6" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3838,13 +3848,13 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1">
         <v>0.55559999999999998</v>
       </c>
       <c r="F2" s="3">
-        <v>-5</v>
+        <v>-3.4443999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3858,13 +3868,13 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1">
         <v>0.75</v>
       </c>
       <c r="F3" s="3">
-        <v>-6.5</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3878,13 +3888,13 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1">
         <v>0.52780000000000005</v>
       </c>
       <c r="F4" s="3">
-        <v>-2.6389</v>
+        <v>-1.75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3898,13 +3908,13 @@
         <v>6684</v>
       </c>
       <c r="D5">
-        <v>538</v>
+        <v>406</v>
       </c>
       <c r="E5" s="1">
         <v>0.44890000000000002</v>
       </c>
       <c r="F5" s="3">
-        <v>0.40450000000000003</v>
+        <v>0.41539999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3918,13 +3928,13 @@
         <v>84787</v>
       </c>
       <c r="D6">
-        <v>651</v>
+        <v>507</v>
       </c>
       <c r="E6" s="1">
         <v>0.4425</v>
       </c>
       <c r="F6" s="3">
-        <v>0.43819999999999998</v>
+        <v>0.43919999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>